<commit_message>
Modélisation - Statut d'un évènement et d'une évaluation (#352)
* Update sfe_modelisation_contenu.md

* Update sfe_modelisation_contenu.md

* Update sfe_modelisation_contenu.md

* Update sfe_modelisation_contenu.md

* Update sfe_modelisation_contenu.md fde038d696e4debf9611f6649179098b1a746019
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tddui-admission-date.xlsx
+++ b/main/ig/StructureDefinition-tddui-admission-date.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-01T06:49:21+00:00</t>
+    <t>2025-09-10T13:27:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -664,42 +664,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="19.59765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.80078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.80078125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="10.04296875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.609375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.6640625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.4296875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="21.57421875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="19.625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="18.1875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="16.828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="36.0390625" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="15.59375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="24.98046875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="21.4140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>